<commit_message>
Fixed issues with databases by country not getting uploaded.  New database for indicator mappings.
</commit_message>
<xml_diff>
--- a/SourceData/budgetmapping/BGModData.xlsx
+++ b/SourceData/budgetmapping/BGModData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\budgetmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDFF959-DEE7-4736-B197-34A45EF7724F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FA2D8-60AD-4EE0-9D7D-54A76BDE570F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3416,10 +3416,10 @@
     <t>Actiivity</t>
   </si>
   <si>
-    <t>1, 2, 3</t>
-  </si>
-  <si>
-    <t>Drugs/Supplies, Labor, Visits</t>
+    <t>2, 3, 4</t>
+  </si>
+  <si>
+    <t>Interventions, Labor, Visits</t>
   </si>
 </sst>
 </file>
@@ -9584,9 +9584,9 @@
   <dimension ref="A1:R454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="P395" sqref="P395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added medical equipment indicator mappings for TB for Budget Mapping.
</commit_message>
<xml_diff>
--- a/SourceData/budgetmapping/BGModData.xlsx
+++ b/SourceData/budgetmapping/BGModData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\budgetmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FA2D8-60AD-4EE0-9D7D-54A76BDE570F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A79CE49-7389-4982-97BF-90BF75CBFABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BudgetDB" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4539" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4581" uniqueCount="1135">
   <si>
     <t>TG_AggregateConstant</t>
   </si>
@@ -3413,13 +3413,40 @@
     <t>&lt;Indicator Type ID&gt;</t>
   </si>
   <si>
-    <t>Actiivity</t>
-  </si>
-  <si>
     <t>2, 3, 4</t>
   </si>
   <si>
     <t>Interventions, Labor, Visits</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Medical equipment</t>
+  </si>
+  <si>
+    <t>Health post</t>
+  </si>
+  <si>
+    <t>Prehospital emergency</t>
+  </si>
+  <si>
+    <t>Health centre</t>
+  </si>
+  <si>
+    <t>District/General hospital</t>
+  </si>
+  <si>
+    <t>National/Regional/Provincial hospital</t>
+  </si>
+  <si>
+    <t>Free-standing general outpatient clinic</t>
+  </si>
+  <si>
+    <t>Free-standing specialized outpatient clinic</t>
   </si>
 </sst>
 </file>
@@ -4291,7 +4318,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -5161,7 +5188,7 @@
   <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
@@ -9584,9 +9611,9 @@
   <dimension ref="A1:R454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="P395" sqref="P395"/>
+      <selection pane="bottomLeft" activeCell="P410" sqref="P410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9678,7 +9705,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -9728,7 +9755,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -9778,7 +9805,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -9828,7 +9855,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -9878,7 +9905,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -9928,7 +9955,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -9978,7 +10005,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -10028,7 +10055,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -10078,7 +10105,7 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -10128,7 +10155,7 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -10178,7 +10205,7 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K12">
         <v>2</v>
@@ -10228,7 +10255,7 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -10278,7 +10305,7 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K14">
         <v>2</v>
@@ -10328,7 +10355,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K15">
         <v>2</v>
@@ -10378,7 +10405,7 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -10428,7 +10455,7 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -10478,7 +10505,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K18">
         <v>2</v>
@@ -10528,7 +10555,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K19">
         <v>2</v>
@@ -10578,7 +10605,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K20">
         <v>2</v>
@@ -10628,7 +10655,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -10678,7 +10705,7 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -10728,7 +10755,7 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K23">
         <v>2</v>
@@ -10778,7 +10805,7 @@
         <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K24">
         <v>2</v>
@@ -10828,7 +10855,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -10878,7 +10905,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K26">
         <v>2</v>
@@ -10928,7 +10955,7 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K27">
         <v>2</v>
@@ -10978,7 +11005,7 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K28">
         <v>2</v>
@@ -11028,7 +11055,7 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K29">
         <v>2</v>
@@ -11078,7 +11105,7 @@
         <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -11128,7 +11155,7 @@
         <v>3</v>
       </c>
       <c r="H31" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -11178,7 +11205,7 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -11228,7 +11255,7 @@
         <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -11278,7 +11305,7 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K34">
         <v>2</v>
@@ -11328,7 +11355,7 @@
         <v>3</v>
       </c>
       <c r="H35" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K35">
         <v>2</v>
@@ -11378,7 +11405,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K36">
         <v>2</v>
@@ -11428,7 +11455,7 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K37">
         <v>2</v>
@@ -11478,7 +11505,7 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K38">
         <v>2</v>
@@ -11528,7 +11555,7 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K39">
         <v>2</v>
@@ -11578,7 +11605,7 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K40">
         <v>2</v>
@@ -11628,7 +11655,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K41">
         <v>2</v>
@@ -11678,7 +11705,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K42">
         <v>2</v>
@@ -11728,7 +11755,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K43">
         <v>2</v>
@@ -11778,7 +11805,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -11828,7 +11855,7 @@
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -11878,7 +11905,7 @@
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K46">
         <v>2</v>
@@ -11928,7 +11955,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K47">
         <v>2</v>
@@ -11978,7 +12005,7 @@
         <v>3</v>
       </c>
       <c r="H48" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -12028,7 +12055,7 @@
         <v>3</v>
       </c>
       <c r="H49" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -12078,7 +12105,7 @@
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K50">
         <v>2</v>
@@ -12128,7 +12155,7 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K51">
         <v>2</v>
@@ -12178,7 +12205,7 @@
         <v>3</v>
       </c>
       <c r="H52" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K52">
         <v>2</v>
@@ -12228,7 +12255,7 @@
         <v>3</v>
       </c>
       <c r="H53" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K53">
         <v>2</v>
@@ -12278,7 +12305,7 @@
         <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K54">
         <v>2</v>
@@ -12328,7 +12355,7 @@
         <v>3</v>
       </c>
       <c r="H55" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K55">
         <v>2</v>
@@ -12378,7 +12405,7 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K56">
         <v>2</v>
@@ -12428,7 +12455,7 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K57">
         <v>2</v>
@@ -12478,7 +12505,7 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K58">
         <v>2</v>
@@ -12528,7 +12555,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K59">
         <v>2</v>
@@ -12578,7 +12605,7 @@
         <v>3</v>
       </c>
       <c r="H60" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K60">
         <v>2</v>
@@ -12628,7 +12655,7 @@
         <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K61">
         <v>2</v>
@@ -12678,7 +12705,7 @@
         <v>3</v>
       </c>
       <c r="H62" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K62">
         <v>2</v>
@@ -12728,7 +12755,7 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K63">
         <v>2</v>
@@ -12778,7 +12805,7 @@
         <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K64">
         <v>2</v>
@@ -12828,7 +12855,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -12878,7 +12905,7 @@
         <v>3</v>
       </c>
       <c r="H66" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K66">
         <v>2</v>
@@ -12928,7 +12955,7 @@
         <v>3</v>
       </c>
       <c r="H67" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K67">
         <v>2</v>
@@ -12978,7 +13005,7 @@
         <v>3</v>
       </c>
       <c r="H68" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K68">
         <v>2</v>
@@ -13028,7 +13055,7 @@
         <v>3</v>
       </c>
       <c r="H69" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K69">
         <v>2</v>
@@ -13078,7 +13105,7 @@
         <v>3</v>
       </c>
       <c r="H70" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K70">
         <v>2</v>
@@ -13128,7 +13155,7 @@
         <v>3</v>
       </c>
       <c r="H71" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K71">
         <v>2</v>
@@ -13178,7 +13205,7 @@
         <v>3</v>
       </c>
       <c r="H72" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K72">
         <v>3</v>
@@ -13228,7 +13255,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K73">
         <v>3</v>
@@ -13278,7 +13305,7 @@
         <v>3</v>
       </c>
       <c r="H74" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K74">
         <v>3</v>
@@ -13328,7 +13355,7 @@
         <v>3</v>
       </c>
       <c r="H75" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K75">
         <v>3</v>
@@ -13378,7 +13405,7 @@
         <v>3</v>
       </c>
       <c r="H76" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K76">
         <v>3</v>
@@ -13428,7 +13455,7 @@
         <v>3</v>
       </c>
       <c r="H77" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K77">
         <v>3</v>
@@ -13478,7 +13505,7 @@
         <v>3</v>
       </c>
       <c r="H78" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K78">
         <v>3</v>
@@ -13528,7 +13555,7 @@
         <v>3</v>
       </c>
       <c r="H79" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K79">
         <v>3</v>
@@ -13578,7 +13605,7 @@
         <v>3</v>
       </c>
       <c r="H80" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K80">
         <v>3</v>
@@ -13628,7 +13655,7 @@
         <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K81">
         <v>3</v>
@@ -13678,7 +13705,7 @@
         <v>3</v>
       </c>
       <c r="H82" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K82">
         <v>3</v>
@@ -13728,7 +13755,7 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K83">
         <v>3</v>
@@ -13778,7 +13805,7 @@
         <v>3</v>
       </c>
       <c r="H84" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K84">
         <v>3</v>
@@ -13828,7 +13855,7 @@
         <v>3</v>
       </c>
       <c r="H85" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K85">
         <v>3</v>
@@ -13878,7 +13905,7 @@
         <v>3</v>
       </c>
       <c r="H86" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K86">
         <v>3</v>
@@ -13928,7 +13955,7 @@
         <v>3</v>
       </c>
       <c r="H87" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K87">
         <v>3</v>
@@ -13978,7 +14005,7 @@
         <v>3</v>
       </c>
       <c r="H88" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K88">
         <v>4</v>
@@ -14028,7 +14055,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K89">
         <v>4</v>
@@ -14078,7 +14105,7 @@
         <v>3</v>
       </c>
       <c r="H90" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K90">
         <v>4</v>
@@ -14128,7 +14155,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K91">
         <v>4</v>
@@ -14178,7 +14205,7 @@
         <v>3</v>
       </c>
       <c r="H92" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K92">
         <v>4</v>
@@ -14228,7 +14255,7 @@
         <v>3</v>
       </c>
       <c r="H93" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K93">
         <v>4</v>
@@ -14278,7 +14305,7 @@
         <v>3</v>
       </c>
       <c r="H94" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K94">
         <v>4</v>
@@ -14328,7 +14355,7 @@
         <v>3</v>
       </c>
       <c r="H95" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K95">
         <v>4</v>
@@ -14378,7 +14405,7 @@
         <v>3</v>
       </c>
       <c r="H96" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K96">
         <v>4</v>
@@ -14428,7 +14455,7 @@
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K97">
         <v>4</v>
@@ -14478,7 +14505,7 @@
         <v>3</v>
       </c>
       <c r="H98" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K98">
         <v>4</v>
@@ -14528,7 +14555,7 @@
         <v>3</v>
       </c>
       <c r="H99" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K99">
         <v>4</v>
@@ -14578,7 +14605,7 @@
         <v>3</v>
       </c>
       <c r="H100" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K100">
         <v>4</v>
@@ -14628,7 +14655,7 @@
         <v>3</v>
       </c>
       <c r="H101" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K101">
         <v>4</v>
@@ -14678,7 +14705,7 @@
         <v>3</v>
       </c>
       <c r="H102" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K102">
         <v>4</v>
@@ -14728,7 +14755,7 @@
         <v>3</v>
       </c>
       <c r="H103" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K103">
         <v>4</v>
@@ -14778,7 +14805,7 @@
         <v>3</v>
       </c>
       <c r="H104" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K104">
         <v>4</v>
@@ -14828,7 +14855,7 @@
         <v>3</v>
       </c>
       <c r="H105" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K105">
         <v>4</v>
@@ -14878,7 +14905,7 @@
         <v>3</v>
       </c>
       <c r="H106" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K106">
         <v>4</v>
@@ -14928,7 +14955,7 @@
         <v>3</v>
       </c>
       <c r="H107" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -14978,7 +15005,7 @@
         <v>3</v>
       </c>
       <c r="H108" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K108">
         <v>4</v>
@@ -15028,7 +15055,7 @@
         <v>3</v>
       </c>
       <c r="H109" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K109">
         <v>4</v>
@@ -15078,7 +15105,7 @@
         <v>3</v>
       </c>
       <c r="H110" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K110">
         <v>4</v>
@@ -15128,7 +15155,7 @@
         <v>3</v>
       </c>
       <c r="H111" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K111">
         <v>4</v>
@@ -15178,7 +15205,7 @@
         <v>3</v>
       </c>
       <c r="H112" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K112">
         <v>4</v>
@@ -15228,7 +15255,7 @@
         <v>3</v>
       </c>
       <c r="H113" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K113">
         <v>4</v>
@@ -15278,7 +15305,7 @@
         <v>3</v>
       </c>
       <c r="H114" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K114">
         <v>4</v>
@@ -15328,7 +15355,7 @@
         <v>3</v>
       </c>
       <c r="H115" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K115">
         <v>4</v>
@@ -15378,7 +15405,7 @@
         <v>3</v>
       </c>
       <c r="H116" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K116">
         <v>4</v>
@@ -15428,7 +15455,7 @@
         <v>3</v>
       </c>
       <c r="H117" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K117">
         <v>4</v>
@@ -15478,7 +15505,7 @@
         <v>3</v>
       </c>
       <c r="H118" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K118">
         <v>4</v>
@@ -15528,7 +15555,7 @@
         <v>3</v>
       </c>
       <c r="H119" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K119">
         <v>4</v>
@@ -15578,7 +15605,7 @@
         <v>3</v>
       </c>
       <c r="H120" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K120">
         <v>4</v>
@@ -15628,7 +15655,7 @@
         <v>3</v>
       </c>
       <c r="H121" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K121">
         <v>4</v>
@@ -15678,7 +15705,7 @@
         <v>3</v>
       </c>
       <c r="H122" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K122">
         <v>4</v>
@@ -15728,7 +15755,7 @@
         <v>3</v>
       </c>
       <c r="H123" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K123">
         <v>4</v>
@@ -15778,7 +15805,7 @@
         <v>3</v>
       </c>
       <c r="H124" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K124">
         <v>4</v>
@@ -15828,7 +15855,7 @@
         <v>3</v>
       </c>
       <c r="H125" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K125">
         <v>4</v>
@@ -15878,7 +15905,7 @@
         <v>3</v>
       </c>
       <c r="H126" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K126">
         <v>4</v>
@@ -15928,7 +15955,7 @@
         <v>3</v>
       </c>
       <c r="H127" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K127">
         <v>4</v>
@@ -15978,7 +16005,7 @@
         <v>3</v>
       </c>
       <c r="H128" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K128">
         <v>4</v>
@@ -16028,7 +16055,7 @@
         <v>3</v>
       </c>
       <c r="H129" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K129">
         <v>4</v>
@@ -16078,7 +16105,7 @@
         <v>3</v>
       </c>
       <c r="H130" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K130">
         <v>4</v>
@@ -16128,7 +16155,7 @@
         <v>3</v>
       </c>
       <c r="H131" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K131">
         <v>4</v>
@@ -16178,7 +16205,7 @@
         <v>3</v>
       </c>
       <c r="H132" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K132">
         <v>4</v>
@@ -16228,7 +16255,7 @@
         <v>3</v>
       </c>
       <c r="H133" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K133">
         <v>4</v>
@@ -16278,7 +16305,7 @@
         <v>3</v>
       </c>
       <c r="H134" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K134">
         <v>4</v>
@@ -16328,7 +16355,7 @@
         <v>3</v>
       </c>
       <c r="H135" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K135">
         <v>4</v>
@@ -16378,7 +16405,7 @@
         <v>3</v>
       </c>
       <c r="H136" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K136">
         <v>4</v>
@@ -16428,7 +16455,7 @@
         <v>3</v>
       </c>
       <c r="H137" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K137">
         <v>4</v>
@@ -16478,7 +16505,7 @@
         <v>3</v>
       </c>
       <c r="H138" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K138">
         <v>4</v>
@@ -16528,7 +16555,7 @@
         <v>3</v>
       </c>
       <c r="H139" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K139">
         <v>4</v>
@@ -16578,7 +16605,7 @@
         <v>3</v>
       </c>
       <c r="H140" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K140">
         <v>4</v>
@@ -16628,7 +16655,7 @@
         <v>3</v>
       </c>
       <c r="H141" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K141">
         <v>4</v>
@@ -16678,7 +16705,7 @@
         <v>3</v>
       </c>
       <c r="H142" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K142">
         <v>4</v>
@@ -16728,7 +16755,7 @@
         <v>3</v>
       </c>
       <c r="H143" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K143">
         <v>4</v>
@@ -16778,7 +16805,7 @@
         <v>3</v>
       </c>
       <c r="H144" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K144">
         <v>4</v>
@@ -16828,7 +16855,7 @@
         <v>3</v>
       </c>
       <c r="H145" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K145">
         <v>4</v>
@@ -16878,7 +16905,7 @@
         <v>3</v>
       </c>
       <c r="H146" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K146">
         <v>4</v>
@@ -16928,7 +16955,7 @@
         <v>3</v>
       </c>
       <c r="H147" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K147">
         <v>4</v>
@@ -16978,7 +17005,7 @@
         <v>3</v>
       </c>
       <c r="H148" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K148">
         <v>4</v>
@@ -17028,7 +17055,7 @@
         <v>3</v>
       </c>
       <c r="H149" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K149">
         <v>5</v>
@@ -17078,7 +17105,7 @@
         <v>3</v>
       </c>
       <c r="H150" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K150">
         <v>5</v>
@@ -17128,7 +17155,7 @@
         <v>3</v>
       </c>
       <c r="H151" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K151">
         <v>5</v>
@@ -17178,7 +17205,7 @@
         <v>3</v>
       </c>
       <c r="H152" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K152">
         <v>5</v>
@@ -17228,7 +17255,7 @@
         <v>3</v>
       </c>
       <c r="H153" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K153">
         <v>5</v>
@@ -17278,7 +17305,7 @@
         <v>3</v>
       </c>
       <c r="H154" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K154">
         <v>5</v>
@@ -17328,7 +17355,7 @@
         <v>3</v>
       </c>
       <c r="H155" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K155">
         <v>5</v>
@@ -17378,7 +17405,7 @@
         <v>3</v>
       </c>
       <c r="H156" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K156">
         <v>5</v>
@@ -17428,7 +17455,7 @@
         <v>3</v>
       </c>
       <c r="H157" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K157">
         <v>5</v>
@@ -17478,7 +17505,7 @@
         <v>3</v>
       </c>
       <c r="H158" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K158">
         <v>5</v>
@@ -17528,7 +17555,7 @@
         <v>3</v>
       </c>
       <c r="H159" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K159">
         <v>5</v>
@@ -17578,7 +17605,7 @@
         <v>3</v>
       </c>
       <c r="H160" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K160">
         <v>5</v>
@@ -17628,7 +17655,7 @@
         <v>3</v>
       </c>
       <c r="H161" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K161">
         <v>5</v>
@@ -17678,7 +17705,7 @@
         <v>3</v>
       </c>
       <c r="H162" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K162">
         <v>5</v>
@@ -17728,7 +17755,7 @@
         <v>3</v>
       </c>
       <c r="H163" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K163">
         <v>5</v>
@@ -17778,7 +17805,7 @@
         <v>3</v>
       </c>
       <c r="H164" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K164">
         <v>5</v>
@@ -17828,7 +17855,7 @@
         <v>3</v>
       </c>
       <c r="H165" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K165">
         <v>5</v>
@@ -17878,7 +17905,7 @@
         <v>3</v>
       </c>
       <c r="H166" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K166">
         <v>5</v>
@@ -17928,7 +17955,7 @@
         <v>3</v>
       </c>
       <c r="H167" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K167">
         <v>5</v>
@@ -17978,7 +18005,7 @@
         <v>3</v>
       </c>
       <c r="H168" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K168">
         <v>5</v>
@@ -18028,7 +18055,7 @@
         <v>3</v>
       </c>
       <c r="H169" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K169">
         <v>5</v>
@@ -18078,7 +18105,7 @@
         <v>3</v>
       </c>
       <c r="H170" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K170">
         <v>5</v>
@@ -18128,7 +18155,7 @@
         <v>3</v>
       </c>
       <c r="H171" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K171">
         <v>5</v>
@@ -18178,7 +18205,7 @@
         <v>3</v>
       </c>
       <c r="H172" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K172">
         <v>6</v>
@@ -18228,7 +18255,7 @@
         <v>3</v>
       </c>
       <c r="H173" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K173">
         <v>6</v>
@@ -18278,7 +18305,7 @@
         <v>3</v>
       </c>
       <c r="H174" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K174">
         <v>6</v>
@@ -18328,7 +18355,7 @@
         <v>3</v>
       </c>
       <c r="H175" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K175">
         <v>6</v>
@@ -18378,7 +18405,7 @@
         <v>3</v>
       </c>
       <c r="H176" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K176">
         <v>7</v>
@@ -18428,7 +18455,7 @@
         <v>3</v>
       </c>
       <c r="H177" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K177">
         <v>7</v>
@@ -18478,7 +18505,7 @@
         <v>3</v>
       </c>
       <c r="H178" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K178">
         <v>7</v>
@@ -18528,7 +18555,7 @@
         <v>3</v>
       </c>
       <c r="H179" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K179">
         <v>7</v>
@@ -18578,7 +18605,7 @@
         <v>3</v>
       </c>
       <c r="H180" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K180">
         <v>7</v>
@@ -18628,7 +18655,7 @@
         <v>3</v>
       </c>
       <c r="H181" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K181">
         <v>7</v>
@@ -18678,7 +18705,7 @@
         <v>3</v>
       </c>
       <c r="H182" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K182">
         <v>8</v>
@@ -18728,7 +18755,7 @@
         <v>3</v>
       </c>
       <c r="H183" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K183">
         <v>8</v>
@@ -18778,7 +18805,7 @@
         <v>3</v>
       </c>
       <c r="H184" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K184">
         <v>8</v>
@@ -18828,7 +18855,7 @@
         <v>3</v>
       </c>
       <c r="H185" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K185">
         <v>8</v>
@@ -18878,7 +18905,7 @@
         <v>3</v>
       </c>
       <c r="H186" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K186">
         <v>8</v>
@@ -18928,7 +18955,7 @@
         <v>3</v>
       </c>
       <c r="H187" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K187">
         <v>8</v>
@@ -18978,7 +19005,7 @@
         <v>3</v>
       </c>
       <c r="H188" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K188">
         <v>8</v>
@@ -19028,7 +19055,7 @@
         <v>3</v>
       </c>
       <c r="H189" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K189">
         <v>8</v>
@@ -19078,7 +19105,7 @@
         <v>3</v>
       </c>
       <c r="H190" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K190">
         <v>8</v>
@@ -19128,7 +19155,7 @@
         <v>3</v>
       </c>
       <c r="H191" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K191">
         <v>9</v>
@@ -19178,7 +19205,7 @@
         <v>3</v>
       </c>
       <c r="H192" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K192">
         <v>9</v>
@@ -19228,7 +19255,7 @@
         <v>3</v>
       </c>
       <c r="H193" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K193">
         <v>9</v>
@@ -19278,7 +19305,7 @@
         <v>3</v>
       </c>
       <c r="H194" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K194">
         <v>9</v>
@@ -19328,7 +19355,7 @@
         <v>3</v>
       </c>
       <c r="H195" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K195">
         <v>9</v>
@@ -19378,7 +19405,7 @@
         <v>3</v>
       </c>
       <c r="H196" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K196">
         <v>9</v>
@@ -19428,7 +19455,7 @@
         <v>3</v>
       </c>
       <c r="H197" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K197">
         <v>9</v>
@@ -19478,7 +19505,7 @@
         <v>3</v>
       </c>
       <c r="H198" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K198">
         <v>9</v>
@@ -19528,7 +19555,7 @@
         <v>3</v>
       </c>
       <c r="H199" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K199">
         <v>9</v>
@@ -19578,7 +19605,7 @@
         <v>3</v>
       </c>
       <c r="H200" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K200">
         <v>9</v>
@@ -19628,7 +19655,7 @@
         <v>3</v>
       </c>
       <c r="H201" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K201">
         <v>9</v>
@@ -19678,7 +19705,7 @@
         <v>3</v>
       </c>
       <c r="H202" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K202">
         <v>9</v>
@@ -19728,7 +19755,7 @@
         <v>3</v>
       </c>
       <c r="H203" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K203">
         <v>9</v>
@@ -19778,7 +19805,7 @@
         <v>3</v>
       </c>
       <c r="H204" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K204">
         <v>9</v>
@@ -19828,7 +19855,7 @@
         <v>3</v>
       </c>
       <c r="H205" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K205">
         <v>9</v>
@@ -19878,7 +19905,7 @@
         <v>3</v>
       </c>
       <c r="H206" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K206">
         <v>9</v>
@@ -19928,7 +19955,7 @@
         <v>3</v>
       </c>
       <c r="H207" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K207">
         <v>9</v>
@@ -19978,7 +20005,7 @@
         <v>3</v>
       </c>
       <c r="H208" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K208">
         <v>9</v>
@@ -20028,7 +20055,7 @@
         <v>3</v>
       </c>
       <c r="H209" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K209">
         <v>9</v>
@@ -20078,7 +20105,7 @@
         <v>3</v>
       </c>
       <c r="H210" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K210">
         <v>9</v>
@@ -20128,7 +20155,7 @@
         <v>3</v>
       </c>
       <c r="H211" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K211">
         <v>9</v>
@@ -20178,7 +20205,7 @@
         <v>3</v>
       </c>
       <c r="H212" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K212">
         <v>9</v>
@@ -20228,7 +20255,7 @@
         <v>3</v>
       </c>
       <c r="H213" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K213">
         <v>9</v>
@@ -20278,7 +20305,7 @@
         <v>3</v>
       </c>
       <c r="H214" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K214">
         <v>9</v>
@@ -20328,7 +20355,7 @@
         <v>3</v>
       </c>
       <c r="H215" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K215">
         <v>9</v>
@@ -20378,7 +20405,7 @@
         <v>3</v>
       </c>
       <c r="H216" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K216">
         <v>9</v>
@@ -20428,7 +20455,7 @@
         <v>3</v>
       </c>
       <c r="H217" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K217">
         <v>9</v>
@@ -20478,7 +20505,7 @@
         <v>3</v>
       </c>
       <c r="H218" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K218">
         <v>9</v>
@@ -20528,7 +20555,7 @@
         <v>3</v>
       </c>
       <c r="H219" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K219">
         <v>9</v>
@@ -20578,7 +20605,7 @@
         <v>3</v>
       </c>
       <c r="H220" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K220">
         <v>9</v>
@@ -20628,7 +20655,7 @@
         <v>3</v>
       </c>
       <c r="H221" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K221">
         <v>9</v>
@@ -20678,7 +20705,7 @@
         <v>3</v>
       </c>
       <c r="H222" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K222">
         <v>9</v>
@@ -20728,7 +20755,7 @@
         <v>3</v>
       </c>
       <c r="H223" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K223">
         <v>9</v>
@@ -20778,7 +20805,7 @@
         <v>3</v>
       </c>
       <c r="H224" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K224">
         <v>9</v>
@@ -20828,7 +20855,7 @@
         <v>3</v>
       </c>
       <c r="H225" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K225">
         <v>9</v>
@@ -20878,7 +20905,7 @@
         <v>3</v>
       </c>
       <c r="H226" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K226">
         <v>9</v>
@@ -20928,7 +20955,7 @@
         <v>3</v>
       </c>
       <c r="H227" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K227">
         <v>9</v>
@@ -20978,7 +21005,7 @@
         <v>3</v>
       </c>
       <c r="H228" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K228">
         <v>9</v>
@@ -21028,7 +21055,7 @@
         <v>3</v>
       </c>
       <c r="H229" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K229">
         <v>9</v>
@@ -21078,7 +21105,7 @@
         <v>3</v>
       </c>
       <c r="H230" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K230">
         <v>9</v>
@@ -21128,7 +21155,7 @@
         <v>3</v>
       </c>
       <c r="H231" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K231">
         <v>9</v>
@@ -21178,7 +21205,7 @@
         <v>3</v>
       </c>
       <c r="H232" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K232">
         <v>9</v>
@@ -21228,7 +21255,7 @@
         <v>3</v>
       </c>
       <c r="H233" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K233">
         <v>9</v>
@@ -21278,7 +21305,7 @@
         <v>3</v>
       </c>
       <c r="H234" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K234">
         <v>9</v>
@@ -21328,7 +21355,7 @@
         <v>3</v>
       </c>
       <c r="H235" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K235">
         <v>9</v>
@@ -21378,7 +21405,7 @@
         <v>3</v>
       </c>
       <c r="H236" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K236">
         <v>9</v>
@@ -21428,7 +21455,7 @@
         <v>3</v>
       </c>
       <c r="H237" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K237">
         <v>9</v>
@@ -21478,7 +21505,7 @@
         <v>3</v>
       </c>
       <c r="H238" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K238">
         <v>9</v>
@@ -21528,7 +21555,7 @@
         <v>3</v>
       </c>
       <c r="H239" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K239">
         <v>9</v>
@@ -21578,7 +21605,7 @@
         <v>3</v>
       </c>
       <c r="H240" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K240">
         <v>9</v>
@@ -21628,7 +21655,7 @@
         <v>3</v>
       </c>
       <c r="H241" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K241">
         <v>9</v>
@@ -21678,7 +21705,7 @@
         <v>3</v>
       </c>
       <c r="H242" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K242">
         <v>9</v>
@@ -21728,7 +21755,7 @@
         <v>3</v>
       </c>
       <c r="H243" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K243">
         <v>9</v>
@@ -21778,7 +21805,7 @@
         <v>3</v>
       </c>
       <c r="H244" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K244">
         <v>9</v>
@@ -21828,7 +21855,7 @@
         <v>3</v>
       </c>
       <c r="H245" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K245">
         <v>9</v>
@@ -21878,7 +21905,7 @@
         <v>3</v>
       </c>
       <c r="H246" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K246">
         <v>9</v>
@@ -21928,7 +21955,7 @@
         <v>3</v>
       </c>
       <c r="H247" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K247">
         <v>9</v>
@@ -21978,7 +22005,7 @@
         <v>3</v>
       </c>
       <c r="H248" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K248">
         <v>9</v>
@@ -22028,7 +22055,7 @@
         <v>3</v>
       </c>
       <c r="H249" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K249">
         <v>9</v>
@@ -22078,7 +22105,7 @@
         <v>3</v>
       </c>
       <c r="H250" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K250">
         <v>9</v>
@@ -22128,7 +22155,7 @@
         <v>3</v>
       </c>
       <c r="H251" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K251">
         <v>9</v>
@@ -22178,7 +22205,7 @@
         <v>3</v>
       </c>
       <c r="H252" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K252">
         <v>9</v>
@@ -22228,7 +22255,7 @@
         <v>3</v>
       </c>
       <c r="H253" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K253">
         <v>10</v>
@@ -22278,7 +22305,7 @@
         <v>3</v>
       </c>
       <c r="H254" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K254">
         <v>10</v>
@@ -22328,7 +22355,7 @@
         <v>3</v>
       </c>
       <c r="H255" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K255">
         <v>10</v>
@@ -22378,7 +22405,7 @@
         <v>3</v>
       </c>
       <c r="H256" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K256">
         <v>10</v>
@@ -22428,7 +22455,7 @@
         <v>3</v>
       </c>
       <c r="H257" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K257">
         <v>10</v>
@@ -22478,7 +22505,7 @@
         <v>3</v>
       </c>
       <c r="H258" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K258">
         <v>10</v>
@@ -22528,7 +22555,7 @@
         <v>3</v>
       </c>
       <c r="H259" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K259">
         <v>10</v>
@@ -22578,7 +22605,7 @@
         <v>3</v>
       </c>
       <c r="H260" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K260">
         <v>10</v>
@@ -22628,7 +22655,7 @@
         <v>3</v>
       </c>
       <c r="H261" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K261">
         <v>10</v>
@@ -22678,7 +22705,7 @@
         <v>3</v>
       </c>
       <c r="H262" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K262">
         <v>10</v>
@@ -22728,7 +22755,7 @@
         <v>3</v>
       </c>
       <c r="H263" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K263">
         <v>10</v>
@@ -22778,7 +22805,7 @@
         <v>3</v>
       </c>
       <c r="H264" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K264">
         <v>10</v>
@@ -22828,7 +22855,7 @@
         <v>3</v>
       </c>
       <c r="H265" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K265">
         <v>11</v>
@@ -22878,7 +22905,7 @@
         <v>3</v>
       </c>
       <c r="H266" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K266">
         <v>11</v>
@@ -22928,7 +22955,7 @@
         <v>3</v>
       </c>
       <c r="H267" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K267">
         <v>11</v>
@@ -22978,7 +23005,7 @@
         <v>3</v>
       </c>
       <c r="H268" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K268">
         <v>11</v>
@@ -23028,7 +23055,7 @@
         <v>3</v>
       </c>
       <c r="H269" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K269">
         <v>11</v>
@@ -23078,7 +23105,7 @@
         <v>3</v>
       </c>
       <c r="H270" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K270">
         <v>11</v>
@@ -23128,7 +23155,7 @@
         <v>3</v>
       </c>
       <c r="H271" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K271">
         <v>11</v>
@@ -23178,7 +23205,7 @@
         <v>3</v>
       </c>
       <c r="H272" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K272">
         <v>11</v>
@@ -23228,7 +23255,7 @@
         <v>3</v>
       </c>
       <c r="H273" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K273">
         <v>11</v>
@@ -23278,7 +23305,7 @@
         <v>3</v>
       </c>
       <c r="H274" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K274">
         <v>11</v>
@@ -23328,7 +23355,7 @@
         <v>3</v>
       </c>
       <c r="H275" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K275">
         <v>11</v>
@@ -23378,7 +23405,7 @@
         <v>3</v>
       </c>
       <c r="H276" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K276">
         <v>11</v>
@@ -23428,7 +23455,7 @@
         <v>3</v>
       </c>
       <c r="H277" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K277">
         <v>11</v>
@@ -23478,7 +23505,7 @@
         <v>3</v>
       </c>
       <c r="H278" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K278">
         <v>11</v>
@@ -23528,7 +23555,7 @@
         <v>3</v>
       </c>
       <c r="H279" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K279">
         <v>11</v>
@@ -23578,7 +23605,7 @@
         <v>3</v>
       </c>
       <c r="H280" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K280">
         <v>11</v>
@@ -23628,7 +23655,7 @@
         <v>3</v>
       </c>
       <c r="H281" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K281">
         <v>11</v>
@@ -23678,7 +23705,7 @@
         <v>3</v>
       </c>
       <c r="H282" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K282">
         <v>11</v>
@@ -23728,7 +23755,7 @@
         <v>3</v>
       </c>
       <c r="H283" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K283">
         <v>11</v>
@@ -23778,7 +23805,7 @@
         <v>3</v>
       </c>
       <c r="H284" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K284">
         <v>11</v>
@@ -23828,7 +23855,7 @@
         <v>3</v>
       </c>
       <c r="H285" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K285">
         <v>12</v>
@@ -23878,7 +23905,7 @@
         <v>3</v>
       </c>
       <c r="H286" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K286">
         <v>12</v>
@@ -23928,7 +23955,7 @@
         <v>3</v>
       </c>
       <c r="H287" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K287">
         <v>12</v>
@@ -23978,7 +24005,7 @@
         <v>3</v>
       </c>
       <c r="H288" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K288">
         <v>12</v>
@@ -24028,7 +24055,7 @@
         <v>3</v>
       </c>
       <c r="H289" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K289">
         <v>12</v>
@@ -24078,7 +24105,7 @@
         <v>3</v>
       </c>
       <c r="H290" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K290">
         <v>12</v>
@@ -24128,7 +24155,7 @@
         <v>3</v>
       </c>
       <c r="H291" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K291">
         <v>12</v>
@@ -24178,7 +24205,7 @@
         <v>3</v>
       </c>
       <c r="H292" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K292">
         <v>12</v>
@@ -24228,7 +24255,7 @@
         <v>3</v>
       </c>
       <c r="H293" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K293">
         <v>12</v>
@@ -24278,7 +24305,7 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K294">
         <v>12</v>
@@ -24328,7 +24355,7 @@
         <v>3</v>
       </c>
       <c r="H295" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K295">
         <v>12</v>
@@ -24378,7 +24405,7 @@
         <v>3</v>
       </c>
       <c r="H296" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K296">
         <v>12</v>
@@ -24428,7 +24455,7 @@
         <v>3</v>
       </c>
       <c r="H297" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K297">
         <v>12</v>
@@ -24478,7 +24505,7 @@
         <v>3</v>
       </c>
       <c r="H298" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K298">
         <v>12</v>
@@ -24528,7 +24555,7 @@
         <v>3</v>
       </c>
       <c r="H299" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K299">
         <v>12</v>
@@ -24578,7 +24605,7 @@
         <v>3</v>
       </c>
       <c r="H300" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K300">
         <v>12</v>
@@ -24628,7 +24655,7 @@
         <v>3</v>
       </c>
       <c r="H301" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K301">
         <v>12</v>
@@ -24678,7 +24705,7 @@
         <v>3</v>
       </c>
       <c r="H302" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K302">
         <v>12</v>
@@ -24728,7 +24755,7 @@
         <v>3</v>
       </c>
       <c r="H303" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K303">
         <v>12</v>
@@ -24778,7 +24805,7 @@
         <v>3</v>
       </c>
       <c r="H304" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K304">
         <v>12</v>
@@ -24828,7 +24855,7 @@
         <v>3</v>
       </c>
       <c r="H305" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K305">
         <v>12</v>
@@ -24878,7 +24905,7 @@
         <v>3</v>
       </c>
       <c r="H306" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K306">
         <v>12</v>
@@ -24928,7 +24955,7 @@
         <v>3</v>
       </c>
       <c r="H307" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K307">
         <v>12</v>
@@ -24978,7 +25005,7 @@
         <v>3</v>
       </c>
       <c r="H308" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K308">
         <v>12</v>
@@ -25028,7 +25055,7 @@
         <v>3</v>
       </c>
       <c r="H309" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K309">
         <v>12</v>
@@ -25078,7 +25105,7 @@
         <v>3</v>
       </c>
       <c r="H310" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K310">
         <v>12</v>
@@ -25128,7 +25155,7 @@
         <v>3</v>
       </c>
       <c r="H311" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K311">
         <v>12</v>
@@ -25178,7 +25205,7 @@
         <v>3</v>
       </c>
       <c r="H312" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K312">
         <v>12</v>
@@ -25228,7 +25255,7 @@
         <v>3</v>
       </c>
       <c r="H313" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K313">
         <v>12</v>
@@ -25278,7 +25305,7 @@
         <v>3</v>
       </c>
       <c r="H314" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K314">
         <v>12</v>
@@ -25328,7 +25355,7 @@
         <v>3</v>
       </c>
       <c r="H315" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K315">
         <v>12</v>
@@ -25378,7 +25405,7 @@
         <v>3</v>
       </c>
       <c r="H316" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K316">
         <v>12</v>
@@ -25428,7 +25455,7 @@
         <v>3</v>
       </c>
       <c r="H317" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K317">
         <v>12</v>
@@ -25478,7 +25505,7 @@
         <v>3</v>
       </c>
       <c r="H318" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K318">
         <v>12</v>
@@ -25528,7 +25555,7 @@
         <v>3</v>
       </c>
       <c r="H319" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K319">
         <v>12</v>
@@ -25578,7 +25605,7 @@
         <v>3</v>
       </c>
       <c r="H320" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K320">
         <v>12</v>
@@ -25628,7 +25655,7 @@
         <v>3</v>
       </c>
       <c r="H321" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K321">
         <v>12</v>
@@ -25678,7 +25705,7 @@
         <v>3</v>
       </c>
       <c r="H322" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K322">
         <v>12</v>
@@ -25728,7 +25755,7 @@
         <v>3</v>
       </c>
       <c r="H323" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K323">
         <v>12</v>
@@ -25778,7 +25805,7 @@
         <v>3</v>
       </c>
       <c r="H324" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K324">
         <v>12</v>
@@ -25828,7 +25855,7 @@
         <v>3</v>
       </c>
       <c r="H325" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K325">
         <v>12</v>
@@ -25878,7 +25905,7 @@
         <v>3</v>
       </c>
       <c r="H326" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K326">
         <v>12</v>
@@ -25928,7 +25955,7 @@
         <v>3</v>
       </c>
       <c r="H327" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K327">
         <v>12</v>
@@ -25978,7 +26005,7 @@
         <v>3</v>
       </c>
       <c r="H328" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K328">
         <v>12</v>
@@ -26028,7 +26055,7 @@
         <v>3</v>
       </c>
       <c r="H329" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K329">
         <v>12</v>
@@ -26078,7 +26105,7 @@
         <v>3</v>
       </c>
       <c r="H330" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K330">
         <v>12</v>
@@ -26128,7 +26155,7 @@
         <v>3</v>
       </c>
       <c r="H331" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K331">
         <v>12</v>
@@ -26178,7 +26205,7 @@
         <v>3</v>
       </c>
       <c r="H332" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K332">
         <v>12</v>
@@ -26228,7 +26255,7 @@
         <v>3</v>
       </c>
       <c r="H333" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K333">
         <v>12</v>
@@ -26278,7 +26305,7 @@
         <v>3</v>
       </c>
       <c r="H334" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K334">
         <v>12</v>
@@ -26328,7 +26355,7 @@
         <v>3</v>
       </c>
       <c r="H335" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K335">
         <v>12</v>
@@ -26378,7 +26405,7 @@
         <v>3</v>
       </c>
       <c r="H336" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K336">
         <v>12</v>
@@ -26428,7 +26455,7 @@
         <v>3</v>
       </c>
       <c r="H337" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K337">
         <v>12</v>
@@ -26478,7 +26505,7 @@
         <v>3</v>
       </c>
       <c r="H338" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K338">
         <v>12</v>
@@ -26528,7 +26555,7 @@
         <v>3</v>
       </c>
       <c r="H339" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K339">
         <v>12</v>
@@ -26578,7 +26605,7 @@
         <v>3</v>
       </c>
       <c r="H340" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K340">
         <v>12</v>
@@ -26628,7 +26655,7 @@
         <v>3</v>
       </c>
       <c r="H341" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K341">
         <v>12</v>
@@ -26678,7 +26705,7 @@
         <v>3</v>
       </c>
       <c r="H342" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="K342">
         <v>12</v>
@@ -26725,10 +26752,10 @@
         <v>629</v>
       </c>
       <c r="G343" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H343" t="s">
         <v>1124</v>
-      </c>
-      <c r="H343" t="s">
-        <v>1125</v>
       </c>
       <c r="I343">
         <v>641</v>
@@ -26763,10 +26790,10 @@
         <v>629</v>
       </c>
       <c r="G344" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H344" t="s">
         <v>1124</v>
-      </c>
-      <c r="H344" t="s">
-        <v>1125</v>
       </c>
       <c r="I344">
         <v>549</v>
@@ -26801,10 +26828,10 @@
         <v>629</v>
       </c>
       <c r="G345" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H345" t="s">
         <v>1124</v>
-      </c>
-      <c r="H345" t="s">
-        <v>1125</v>
       </c>
       <c r="I345">
         <v>550</v>
@@ -26839,10 +26866,10 @@
         <v>629</v>
       </c>
       <c r="G346" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H346" t="s">
         <v>1124</v>
-      </c>
-      <c r="H346" t="s">
-        <v>1125</v>
       </c>
       <c r="I346">
         <v>551</v>
@@ -26877,10 +26904,10 @@
         <v>629</v>
       </c>
       <c r="G347" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H347" t="s">
         <v>1124</v>
-      </c>
-      <c r="H347" t="s">
-        <v>1125</v>
       </c>
       <c r="I347">
         <v>552</v>
@@ -26915,10 +26942,10 @@
         <v>629</v>
       </c>
       <c r="G348" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H348" t="s">
         <v>1124</v>
-      </c>
-      <c r="H348" t="s">
-        <v>1125</v>
       </c>
       <c r="I348">
         <v>553</v>
@@ -26953,10 +26980,10 @@
         <v>629</v>
       </c>
       <c r="G349" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H349" t="s">
         <v>1124</v>
-      </c>
-      <c r="H349" t="s">
-        <v>1125</v>
       </c>
       <c r="I349">
         <v>554</v>
@@ -26991,10 +27018,10 @@
         <v>629</v>
       </c>
       <c r="G350" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H350" t="s">
         <v>1124</v>
-      </c>
-      <c r="H350" t="s">
-        <v>1125</v>
       </c>
       <c r="I350">
         <v>555</v>
@@ -27029,10 +27056,10 @@
         <v>629</v>
       </c>
       <c r="G351" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H351" t="s">
         <v>1124</v>
-      </c>
-      <c r="H351" t="s">
-        <v>1125</v>
       </c>
       <c r="I351">
         <v>556</v>
@@ -27067,10 +27094,10 @@
         <v>629</v>
       </c>
       <c r="G352" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H352" t="s">
         <v>1124</v>
-      </c>
-      <c r="H352" t="s">
-        <v>1125</v>
       </c>
       <c r="I352">
         <v>557</v>
@@ -27105,10 +27132,10 @@
         <v>629</v>
       </c>
       <c r="G353" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H353" t="s">
         <v>1124</v>
-      </c>
-      <c r="H353" t="s">
-        <v>1125</v>
       </c>
       <c r="I353">
         <v>558</v>
@@ -27143,10 +27170,10 @@
         <v>629</v>
       </c>
       <c r="G354" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H354" t="s">
         <v>1124</v>
-      </c>
-      <c r="H354" t="s">
-        <v>1125</v>
       </c>
       <c r="I354">
         <v>559</v>
@@ -27181,10 +27208,10 @@
         <v>629</v>
       </c>
       <c r="G355" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H355" t="s">
         <v>1124</v>
-      </c>
-      <c r="H355" t="s">
-        <v>1125</v>
       </c>
       <c r="I355">
         <v>560</v>
@@ -27219,10 +27246,10 @@
         <v>629</v>
       </c>
       <c r="G356" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H356" t="s">
         <v>1124</v>
-      </c>
-      <c r="H356" t="s">
-        <v>1125</v>
       </c>
       <c r="I356">
         <v>561</v>
@@ -27257,10 +27284,10 @@
         <v>629</v>
       </c>
       <c r="G357" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H357" t="s">
         <v>1124</v>
-      </c>
-      <c r="H357" t="s">
-        <v>1125</v>
       </c>
       <c r="I357">
         <v>562</v>
@@ -27295,10 +27322,10 @@
         <v>629</v>
       </c>
       <c r="G358" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H358" t="s">
         <v>1124</v>
-      </c>
-      <c r="H358" t="s">
-        <v>1125</v>
       </c>
       <c r="I358">
         <v>563</v>
@@ -27333,10 +27360,10 @@
         <v>629</v>
       </c>
       <c r="G359" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H359" t="s">
         <v>1124</v>
-      </c>
-      <c r="H359" t="s">
-        <v>1125</v>
       </c>
       <c r="I359">
         <v>564</v>
@@ -27371,10 +27398,10 @@
         <v>629</v>
       </c>
       <c r="G360" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H360" t="s">
         <v>1124</v>
-      </c>
-      <c r="H360" t="s">
-        <v>1125</v>
       </c>
       <c r="I360">
         <v>565</v>
@@ -27409,10 +27436,10 @@
         <v>629</v>
       </c>
       <c r="G361" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H361" t="s">
         <v>1124</v>
-      </c>
-      <c r="H361" t="s">
-        <v>1125</v>
       </c>
       <c r="I361">
         <v>650</v>
@@ -27447,10 +27474,10 @@
         <v>629</v>
       </c>
       <c r="G362" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H362" t="s">
         <v>1124</v>
-      </c>
-      <c r="H362" t="s">
-        <v>1125</v>
       </c>
       <c r="I362">
         <v>567</v>
@@ -27485,10 +27512,10 @@
         <v>629</v>
       </c>
       <c r="G363" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H363" t="s">
         <v>1124</v>
-      </c>
-      <c r="H363" t="s">
-        <v>1125</v>
       </c>
       <c r="I363">
         <v>569</v>
@@ -27523,10 +27550,10 @@
         <v>629</v>
       </c>
       <c r="G364" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H364" t="s">
         <v>1124</v>
-      </c>
-      <c r="H364" t="s">
-        <v>1125</v>
       </c>
       <c r="I364">
         <v>570</v>
@@ -27561,10 +27588,10 @@
         <v>629</v>
       </c>
       <c r="G365" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H365" t="s">
         <v>1124</v>
-      </c>
-      <c r="H365" t="s">
-        <v>1125</v>
       </c>
       <c r="I365">
         <v>571</v>
@@ -27599,10 +27626,10 @@
         <v>629</v>
       </c>
       <c r="G366" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H366" t="s">
         <v>1124</v>
-      </c>
-      <c r="H366" t="s">
-        <v>1125</v>
       </c>
       <c r="I366">
         <v>572</v>
@@ -27637,10 +27664,10 @@
         <v>629</v>
       </c>
       <c r="G367" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H367" t="s">
         <v>1124</v>
-      </c>
-      <c r="H367" t="s">
-        <v>1125</v>
       </c>
       <c r="I367">
         <v>573</v>
@@ -27675,10 +27702,10 @@
         <v>629</v>
       </c>
       <c r="G368" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H368" t="s">
         <v>1124</v>
-      </c>
-      <c r="H368" t="s">
-        <v>1125</v>
       </c>
       <c r="I368">
         <v>574</v>
@@ -27713,10 +27740,10 @@
         <v>629</v>
       </c>
       <c r="G369" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H369" t="s">
         <v>1124</v>
-      </c>
-      <c r="H369" t="s">
-        <v>1125</v>
       </c>
       <c r="I369">
         <v>575</v>
@@ -27751,10 +27778,10 @@
         <v>629</v>
       </c>
       <c r="G370" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H370" t="s">
         <v>1124</v>
-      </c>
-      <c r="H370" t="s">
-        <v>1125</v>
       </c>
       <c r="I370">
         <v>576</v>
@@ -27789,10 +27816,10 @@
         <v>629</v>
       </c>
       <c r="G371" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H371" t="s">
         <v>1124</v>
-      </c>
-      <c r="H371" t="s">
-        <v>1125</v>
       </c>
       <c r="I371">
         <v>577</v>
@@ -27827,10 +27854,10 @@
         <v>629</v>
       </c>
       <c r="G372" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H372" t="s">
         <v>1124</v>
-      </c>
-      <c r="H372" t="s">
-        <v>1125</v>
       </c>
       <c r="I372">
         <v>578</v>
@@ -27865,10 +27892,10 @@
         <v>629</v>
       </c>
       <c r="G373" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H373" t="s">
         <v>1124</v>
-      </c>
-      <c r="H373" t="s">
-        <v>1125</v>
       </c>
       <c r="I373">
         <v>579</v>
@@ -27903,10 +27930,10 @@
         <v>629</v>
       </c>
       <c r="G374" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H374" t="s">
         <v>1124</v>
-      </c>
-      <c r="H374" t="s">
-        <v>1125</v>
       </c>
       <c r="I374">
         <v>580</v>
@@ -27941,10 +27968,10 @@
         <v>629</v>
       </c>
       <c r="G375" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H375" t="s">
         <v>1124</v>
-      </c>
-      <c r="H375" t="s">
-        <v>1125</v>
       </c>
       <c r="I375">
         <v>581</v>
@@ -27979,10 +28006,10 @@
         <v>629</v>
       </c>
       <c r="G376" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H376" t="s">
         <v>1124</v>
-      </c>
-      <c r="H376" t="s">
-        <v>1125</v>
       </c>
       <c r="I376">
         <v>582</v>
@@ -28017,10 +28044,10 @@
         <v>629</v>
       </c>
       <c r="G377" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H377" t="s">
         <v>1124</v>
-      </c>
-      <c r="H377" t="s">
-        <v>1125</v>
       </c>
       <c r="I377">
         <v>583</v>
@@ -28055,10 +28082,10 @@
         <v>629</v>
       </c>
       <c r="G378" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H378" t="s">
         <v>1124</v>
-      </c>
-      <c r="H378" t="s">
-        <v>1125</v>
       </c>
       <c r="I378">
         <v>584</v>
@@ -28093,10 +28120,10 @@
         <v>629</v>
       </c>
       <c r="G379" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H379" t="s">
         <v>1124</v>
-      </c>
-      <c r="H379" t="s">
-        <v>1125</v>
       </c>
       <c r="I379">
         <v>585</v>
@@ -28131,10 +28158,10 @@
         <v>629</v>
       </c>
       <c r="G380" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H380" t="s">
         <v>1124</v>
-      </c>
-      <c r="H380" t="s">
-        <v>1125</v>
       </c>
       <c r="I380">
         <v>586</v>
@@ -28169,10 +28196,10 @@
         <v>629</v>
       </c>
       <c r="G381" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H381" t="s">
         <v>1124</v>
-      </c>
-      <c r="H381" t="s">
-        <v>1125</v>
       </c>
       <c r="I381">
         <v>649</v>
@@ -28207,10 +28234,10 @@
         <v>629</v>
       </c>
       <c r="G382" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H382" t="s">
         <v>1124</v>
-      </c>
-      <c r="H382" t="s">
-        <v>1125</v>
       </c>
       <c r="I382">
         <v>597</v>
@@ -28245,10 +28272,10 @@
         <v>629</v>
       </c>
       <c r="G383" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H383" t="s">
         <v>1124</v>
-      </c>
-      <c r="H383" t="s">
-        <v>1125</v>
       </c>
       <c r="I383">
         <v>598</v>
@@ -28283,10 +28310,10 @@
         <v>629</v>
       </c>
       <c r="G384" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H384" t="s">
         <v>1124</v>
-      </c>
-      <c r="H384" t="s">
-        <v>1125</v>
       </c>
       <c r="I384">
         <v>599</v>
@@ -28321,10 +28348,10 @@
         <v>629</v>
       </c>
       <c r="G385" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H385" t="s">
         <v>1124</v>
-      </c>
-      <c r="H385" t="s">
-        <v>1125</v>
       </c>
       <c r="I385">
         <v>600</v>
@@ -28359,10 +28386,10 @@
         <v>629</v>
       </c>
       <c r="G386" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H386" t="s">
         <v>1124</v>
-      </c>
-      <c r="H386" t="s">
-        <v>1125</v>
       </c>
       <c r="I386">
         <v>601</v>
@@ -28397,10 +28424,10 @@
         <v>629</v>
       </c>
       <c r="G387" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H387" t="s">
         <v>1124</v>
-      </c>
-      <c r="H387" t="s">
-        <v>1125</v>
       </c>
       <c r="I387">
         <v>602</v>
@@ -28435,10 +28462,10 @@
         <v>629</v>
       </c>
       <c r="G388" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H388" t="s">
         <v>1124</v>
-      </c>
-      <c r="H388" t="s">
-        <v>1125</v>
       </c>
       <c r="I388">
         <v>603</v>
@@ -28473,10 +28500,10 @@
         <v>629</v>
       </c>
       <c r="G389" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H389" t="s">
         <v>1124</v>
-      </c>
-      <c r="H389" t="s">
-        <v>1125</v>
       </c>
       <c r="I389">
         <v>604</v>
@@ -28511,10 +28538,10 @@
         <v>629</v>
       </c>
       <c r="G390" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H390" t="s">
         <v>1124</v>
-      </c>
-      <c r="H390" t="s">
-        <v>1125</v>
       </c>
       <c r="I390">
         <v>605</v>
@@ -28549,10 +28576,10 @@
         <v>629</v>
       </c>
       <c r="G391" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H391" t="s">
         <v>1124</v>
-      </c>
-      <c r="H391" t="s">
-        <v>1125</v>
       </c>
       <c r="I391">
         <v>606</v>
@@ -28587,10 +28614,10 @@
         <v>629</v>
       </c>
       <c r="G392" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H392" t="s">
         <v>1124</v>
-      </c>
-      <c r="H392" t="s">
-        <v>1125</v>
       </c>
       <c r="I392">
         <v>607</v>
@@ -28625,10 +28652,10 @@
         <v>629</v>
       </c>
       <c r="G393" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H393" t="s">
         <v>1124</v>
-      </c>
-      <c r="H393" t="s">
-        <v>1125</v>
       </c>
       <c r="I393">
         <v>608</v>
@@ -28663,10 +28690,10 @@
         <v>629</v>
       </c>
       <c r="G394" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H394" t="s">
         <v>1124</v>
-      </c>
-      <c r="H394" t="s">
-        <v>1125</v>
       </c>
       <c r="I394">
         <v>609</v>
@@ -28701,10 +28728,10 @@
         <v>629</v>
       </c>
       <c r="G395" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H395" t="s">
         <v>1124</v>
-      </c>
-      <c r="H395" t="s">
-        <v>1125</v>
       </c>
       <c r="I395">
         <v>610</v>
@@ -28739,10 +28766,10 @@
         <v>629</v>
       </c>
       <c r="G396" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H396" t="s">
         <v>1124</v>
-      </c>
-      <c r="H396" t="s">
-        <v>1125</v>
       </c>
       <c r="I396">
         <v>611</v>
@@ -28777,10 +28804,10 @@
         <v>629</v>
       </c>
       <c r="G397" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H397" t="s">
         <v>1124</v>
-      </c>
-      <c r="H397" t="s">
-        <v>1125</v>
       </c>
       <c r="I397">
         <v>612</v>
@@ -28815,10 +28842,10 @@
         <v>629</v>
       </c>
       <c r="G398" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H398" t="s">
         <v>1124</v>
-      </c>
-      <c r="H398" t="s">
-        <v>1125</v>
       </c>
       <c r="I398">
         <v>613</v>
@@ -28853,10 +28880,10 @@
         <v>629</v>
       </c>
       <c r="G399" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H399" t="s">
         <v>1124</v>
-      </c>
-      <c r="H399" t="s">
-        <v>1125</v>
       </c>
       <c r="I399">
         <v>614</v>
@@ -28891,10 +28918,10 @@
         <v>629</v>
       </c>
       <c r="G400" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H400" t="s">
         <v>1124</v>
-      </c>
-      <c r="H400" t="s">
-        <v>1125</v>
       </c>
       <c r="I400">
         <v>615</v>
@@ -28929,10 +28956,10 @@
         <v>629</v>
       </c>
       <c r="G401" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H401" t="s">
         <v>1124</v>
-      </c>
-      <c r="H401" t="s">
-        <v>1125</v>
       </c>
       <c r="I401">
         <v>616</v>
@@ -28967,10 +28994,10 @@
         <v>629</v>
       </c>
       <c r="G402" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H402" t="s">
         <v>1124</v>
-      </c>
-      <c r="H402" t="s">
-        <v>1125</v>
       </c>
       <c r="I402">
         <v>617</v>
@@ -29005,10 +29032,10 @@
         <v>629</v>
       </c>
       <c r="G403" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H403" t="s">
         <v>1124</v>
-      </c>
-      <c r="H403" t="s">
-        <v>1125</v>
       </c>
       <c r="I403">
         <v>618</v>
@@ -29043,10 +29070,10 @@
         <v>629</v>
       </c>
       <c r="G404" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H404" t="s">
         <v>1124</v>
-      </c>
-      <c r="H404" t="s">
-        <v>1125</v>
       </c>
       <c r="I404">
         <v>619</v>
@@ -29081,10 +29108,10 @@
         <v>629</v>
       </c>
       <c r="G405" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H405" t="s">
         <v>1124</v>
-      </c>
-      <c r="H405" t="s">
-        <v>1125</v>
       </c>
       <c r="I405">
         <v>620</v>
@@ -29119,10 +29146,10 @@
         <v>629</v>
       </c>
       <c r="G406" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H406" t="s">
         <v>1124</v>
-      </c>
-      <c r="H406" t="s">
-        <v>1125</v>
       </c>
       <c r="I406">
         <v>621</v>
@@ -29157,10 +29184,10 @@
         <v>629</v>
       </c>
       <c r="G407" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H407" t="s">
         <v>1124</v>
-      </c>
-      <c r="H407" t="s">
-        <v>1125</v>
       </c>
       <c r="I407">
         <v>622</v>
@@ -29195,10 +29222,10 @@
         <v>629</v>
       </c>
       <c r="G408" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H408" t="s">
         <v>1124</v>
-      </c>
-      <c r="H408" t="s">
-        <v>1125</v>
       </c>
       <c r="I408">
         <v>623</v>
@@ -29233,10 +29260,10 @@
         <v>629</v>
       </c>
       <c r="G409" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H409" t="s">
         <v>1124</v>
-      </c>
-      <c r="H409" t="s">
-        <v>1125</v>
       </c>
       <c r="I409">
         <v>624</v>
@@ -29271,10 +29298,10 @@
         <v>629</v>
       </c>
       <c r="G410" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H410" t="s">
         <v>1124</v>
-      </c>
-      <c r="H410" t="s">
-        <v>1125</v>
       </c>
       <c r="I410">
         <v>625</v>
@@ -29309,10 +29336,10 @@
         <v>629</v>
       </c>
       <c r="G411" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H411" t="s">
         <v>1124</v>
-      </c>
-      <c r="H411" t="s">
-        <v>1125</v>
       </c>
       <c r="I411">
         <v>35</v>
@@ -29347,10 +29374,10 @@
         <v>629</v>
       </c>
       <c r="G412" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H412" t="s">
         <v>1124</v>
-      </c>
-      <c r="H412" t="s">
-        <v>1125</v>
       </c>
       <c r="I412">
         <v>626</v>
@@ -29385,10 +29412,10 @@
         <v>629</v>
       </c>
       <c r="G413" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H413" t="s">
         <v>1124</v>
-      </c>
-      <c r="H413" t="s">
-        <v>1125</v>
       </c>
       <c r="I413">
         <v>627</v>
@@ -29423,10 +29450,10 @@
         <v>629</v>
       </c>
       <c r="G414" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H414" t="s">
         <v>1124</v>
-      </c>
-      <c r="H414" t="s">
-        <v>1125</v>
       </c>
       <c r="I414">
         <v>49</v>
@@ -29439,6 +29466,272 @@
       </c>
       <c r="R414" t="s">
         <v>1045</v>
+      </c>
+    </row>
+    <row r="415" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A415">
+        <v>2</v>
+      </c>
+      <c r="B415" t="s">
+        <v>630</v>
+      </c>
+      <c r="C415">
+        <v>1</v>
+      </c>
+      <c r="D415" t="s">
+        <v>240</v>
+      </c>
+      <c r="E415">
+        <v>20</v>
+      </c>
+      <c r="F415" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G415">
+        <v>4</v>
+      </c>
+      <c r="H415" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I415">
+        <v>1</v>
+      </c>
+      <c r="J415" t="s">
+        <v>1128</v>
+      </c>
+      <c r="Q415">
+        <v>56</v>
+      </c>
+      <c r="R415" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="416" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A416">
+        <v>2</v>
+      </c>
+      <c r="B416" t="s">
+        <v>630</v>
+      </c>
+      <c r="C416">
+        <v>1</v>
+      </c>
+      <c r="D416" t="s">
+        <v>240</v>
+      </c>
+      <c r="E416">
+        <v>20</v>
+      </c>
+      <c r="F416" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G416">
+        <v>4</v>
+      </c>
+      <c r="H416" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I416">
+        <v>2</v>
+      </c>
+      <c r="J416" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Q416">
+        <v>56</v>
+      </c>
+      <c r="R416" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="417" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A417">
+        <v>2</v>
+      </c>
+      <c r="B417" t="s">
+        <v>630</v>
+      </c>
+      <c r="C417">
+        <v>1</v>
+      </c>
+      <c r="D417" t="s">
+        <v>240</v>
+      </c>
+      <c r="E417">
+        <v>20</v>
+      </c>
+      <c r="F417" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G417">
+        <v>4</v>
+      </c>
+      <c r="H417" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I417">
+        <v>3</v>
+      </c>
+      <c r="J417" t="s">
+        <v>1131</v>
+      </c>
+      <c r="Q417">
+        <v>56</v>
+      </c>
+      <c r="R417" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="418" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A418">
+        <v>2</v>
+      </c>
+      <c r="B418" t="s">
+        <v>630</v>
+      </c>
+      <c r="C418">
+        <v>1</v>
+      </c>
+      <c r="D418" t="s">
+        <v>240</v>
+      </c>
+      <c r="E418">
+        <v>20</v>
+      </c>
+      <c r="F418" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G418">
+        <v>4</v>
+      </c>
+      <c r="H418" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I418">
+        <v>4</v>
+      </c>
+      <c r="J418" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Q418">
+        <v>56</v>
+      </c>
+      <c r="R418" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="419" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A419">
+        <v>2</v>
+      </c>
+      <c r="B419" t="s">
+        <v>630</v>
+      </c>
+      <c r="C419">
+        <v>1</v>
+      </c>
+      <c r="D419" t="s">
+        <v>240</v>
+      </c>
+      <c r="E419">
+        <v>20</v>
+      </c>
+      <c r="F419" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G419">
+        <v>4</v>
+      </c>
+      <c r="H419" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I419">
+        <v>6</v>
+      </c>
+      <c r="J419" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Q419">
+        <v>56</v>
+      </c>
+      <c r="R419" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="420" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A420">
+        <v>2</v>
+      </c>
+      <c r="B420" t="s">
+        <v>630</v>
+      </c>
+      <c r="C420">
+        <v>1</v>
+      </c>
+      <c r="D420" t="s">
+        <v>240</v>
+      </c>
+      <c r="E420">
+        <v>20</v>
+      </c>
+      <c r="F420" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G420">
+        <v>4</v>
+      </c>
+      <c r="H420" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I420">
+        <v>7</v>
+      </c>
+      <c r="J420" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q420">
+        <v>56</v>
+      </c>
+      <c r="R420" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="421" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>2</v>
+      </c>
+      <c r="B421" t="s">
+        <v>630</v>
+      </c>
+      <c r="C421">
+        <v>1</v>
+      </c>
+      <c r="D421" t="s">
+        <v>240</v>
+      </c>
+      <c r="E421">
+        <v>20</v>
+      </c>
+      <c r="F421" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G421">
+        <v>4</v>
+      </c>
+      <c r="H421" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I421">
+        <v>8</v>
+      </c>
+      <c r="J421" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Q421">
+        <v>56</v>
+      </c>
+      <c r="R421" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="454" spans="10:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Various fixes to default WHO budget for Budget mapping.
</commit_message>
<xml_diff>
--- a/SourceData/budgetmapping/BGModData.xlsx
+++ b/SourceData/budgetmapping/BGModData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\budgetmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5674B31-915C-4284-A473-F6B277EFFFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE6FE30-314B-4BE2-89E7-D525D13D58DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BudgetDB" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="FundingSourceDB Fake" sheetId="9" r:id="rId9"/>
     <sheet name="Tags" sheetId="1" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8304" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8346" uniqueCount="1161">
   <si>
     <t>TG_AggregateConstant</t>
   </si>
@@ -5297,8 +5297,8 @@
   <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G202" sqref="G202"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E193" sqref="E193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9970,12 +9970,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEB4B75-3B81-4BF7-80FE-92A0D4964378}">
-  <dimension ref="A1:S907"/>
+  <dimension ref="A1:S913"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A886" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="R902" sqref="R902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49041,10 +49041,10 @@
         <v>1089</v>
       </c>
       <c r="Q802" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R802" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="S802"/>
     </row>
@@ -49080,10 +49080,10 @@
         <v>1090</v>
       </c>
       <c r="Q803" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R803" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="S803"/>
     </row>
@@ -49119,10 +49119,10 @@
         <v>1091</v>
       </c>
       <c r="Q804" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R804" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="S804"/>
     </row>
@@ -49158,10 +49158,10 @@
         <v>1092</v>
       </c>
       <c r="Q805" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R805" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="S805"/>
     </row>
@@ -49197,10 +49197,10 @@
         <v>1093</v>
       </c>
       <c r="Q806" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R806" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="S806"/>
     </row>
@@ -53105,8 +53105,269 @@
       <c r="S906"/>
     </row>
     <row r="907" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A907" s="5">
+        <v>2</v>
+      </c>
+      <c r="B907" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C907" s="5">
+        <v>2</v>
+      </c>
+      <c r="D907" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E907" s="5">
+        <v>20</v>
+      </c>
+      <c r="F907" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G907">
+        <v>4</v>
+      </c>
+      <c r="H907" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I907" s="5">
+        <v>1</v>
+      </c>
+      <c r="J907" s="5" t="s">
+        <v>1128</v>
+      </c>
       <c r="Q907">
         <v>1</v>
+      </c>
+      <c r="R907" s="5" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="908" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A908" s="5">
+        <v>2</v>
+      </c>
+      <c r="B908" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C908" s="5">
+        <v>2</v>
+      </c>
+      <c r="D908" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E908" s="5">
+        <v>20</v>
+      </c>
+      <c r="F908" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G908">
+        <v>4</v>
+      </c>
+      <c r="H908" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I908" s="5">
+        <v>2</v>
+      </c>
+      <c r="J908" s="5" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Q908" s="5">
+        <v>2</v>
+      </c>
+      <c r="R908" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="909" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A909" s="5">
+        <v>2</v>
+      </c>
+      <c r="B909" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C909" s="5">
+        <v>2</v>
+      </c>
+      <c r="D909" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E909" s="5">
+        <v>20</v>
+      </c>
+      <c r="F909" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G909">
+        <v>4</v>
+      </c>
+      <c r="H909" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I909" s="5">
+        <v>3</v>
+      </c>
+      <c r="J909" s="5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="Q909" s="5">
+        <v>2</v>
+      </c>
+      <c r="R909" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="910" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A910" s="5">
+        <v>2</v>
+      </c>
+      <c r="B910" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C910" s="5">
+        <v>2</v>
+      </c>
+      <c r="D910" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E910" s="5">
+        <v>20</v>
+      </c>
+      <c r="F910" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G910">
+        <v>4</v>
+      </c>
+      <c r="H910" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I910" s="5">
+        <v>4</v>
+      </c>
+      <c r="J910" s="5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Q910" s="5">
+        <v>2</v>
+      </c>
+      <c r="R910" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="911" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A911" s="5">
+        <v>2</v>
+      </c>
+      <c r="B911" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C911" s="5">
+        <v>2</v>
+      </c>
+      <c r="D911" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E911" s="5">
+        <v>20</v>
+      </c>
+      <c r="F911" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G911">
+        <v>4</v>
+      </c>
+      <c r="H911" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I911" s="5">
+        <v>6</v>
+      </c>
+      <c r="J911" s="5" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Q911" s="5">
+        <v>2</v>
+      </c>
+      <c r="R911" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="912" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A912" s="5">
+        <v>2</v>
+      </c>
+      <c r="B912" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C912" s="5">
+        <v>2</v>
+      </c>
+      <c r="D912" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E912" s="5">
+        <v>20</v>
+      </c>
+      <c r="F912" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G912">
+        <v>4</v>
+      </c>
+      <c r="H912" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I912" s="5">
+        <v>7</v>
+      </c>
+      <c r="J912" s="5" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q912" s="5">
+        <v>2</v>
+      </c>
+      <c r="R912" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="913" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A913" s="5">
+        <v>2</v>
+      </c>
+      <c r="B913" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="C913" s="5">
+        <v>2</v>
+      </c>
+      <c r="D913" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E913" s="5">
+        <v>20</v>
+      </c>
+      <c r="F913" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G913">
+        <v>4</v>
+      </c>
+      <c r="H913" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I913" s="5">
+        <v>8</v>
+      </c>
+      <c r="J913" s="5" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Q913" s="5">
+        <v>2</v>
+      </c>
+      <c r="R913" t="s">
+        <v>1137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>